<commit_message>
linking add_object to data_models
</commit_message>
<xml_diff>
--- a/skoring/utils/datasets/Experience.xlsx
+++ b/skoring/utils/datasets/Experience.xlsx
@@ -5,38 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\htdocs\REPO GITHUB\sistem-skoring-pelatihan-microsoft\skoring\ml\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\htdocs\REPO GITHUB\sistem-skoring-pelatihan-microsoft\skoring\utils\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8103F92-82F4-4D16-80FC-38C7BF1344E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997CBE11-DC68-4D8D-B859-A9AE695BF8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{ED66DA15-7DEA-4F0B-ABC6-A1D850E710CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
-    <t>Event Name  </t>
+    <t>data</t>
   </si>
   <si>
     <t>Workshop Microsoft 365 - Word for Academic Research </t>
@@ -287,10 +273,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DBCCDA46-634D-49B9-960E-D949BAA4C52E}" name="Table1" displayName="Table1" ref="A1:A79" totalsRowShown="0">
-  <autoFilter ref="A1:A79" xr:uid="{DBCCDA46-634D-49B9-960E-D949BAA4C52E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:A79" totalsRowShown="0">
+  <autoFilter ref="A1:A79" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="3" xr3:uid="{1B40E8BA-C18E-4825-A6F0-05759B631499}" name="Event Name  "/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="data"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -592,11 +578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14EF1C2-548F-4333-8357-64699E6B621B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>